<commit_message>
Income and Expense transactions showing in pages, API call to add and delete and download income and expens, adding add expense form
</commit_message>
<xml_diff>
--- a/backend/expense_details.xlsx
+++ b/backend/expense_details.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -418,35 +418,119 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>rent</v>
+        <v>Food</v>
       </c>
       <c r="B2">
-        <v>5000</v>
+        <v>200</v>
       </c>
       <c r="C2" t="str">
-        <v>2025-06-16</v>
+        <v>2025-06-14</v>
       </c>
       <c r="D2" t="str">
-        <v>Rent for room</v>
+        <v>Pizza dinner with friends</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>movie</v>
+        <v>lunch</v>
       </c>
       <c r="B3">
-        <v>350</v>
+        <v>120</v>
       </c>
       <c r="C3" t="str">
-        <v>2025-06-16</v>
+        <v>2025-06-12</v>
       </c>
       <c r="D3" t="str">
-        <v>Movie ticket</v>
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Groceries</v>
+      </c>
+      <c r="B4">
+        <v>2500</v>
+      </c>
+      <c r="C4" t="str">
+        <v>2025-06-10</v>
+      </c>
+      <c r="D4" t="str">
+        <v>Monthly grocery shopping</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Food</v>
+      </c>
+      <c r="B5">
+        <v>500</v>
+      </c>
+      <c r="C5" t="str">
+        <v>2025-06-10</v>
+      </c>
+      <c r="D5" t="str">
+        <v>Lunch at restaurant</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Transport</v>
+      </c>
+      <c r="B6">
+        <v>700</v>
+      </c>
+      <c r="C6" t="str">
+        <v>2025-06-08</v>
+      </c>
+      <c r="D6" t="str">
+        <v>Bus and metro fare</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Ice cream</v>
+      </c>
+      <c r="B7">
+        <v>50</v>
+      </c>
+      <c r="C7" t="str">
+        <v>2025-06-02</v>
+      </c>
+      <c r="D7" t="str">
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Rent</v>
+      </c>
+      <c r="B8">
+        <v>1000</v>
+      </c>
+      <c r="C8" t="str">
+        <v>2025-06-01</v>
+      </c>
+      <c r="D8" t="str">
+        <v>June rent payment</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>Electricity</v>
+      </c>
+      <c r="B9">
+        <v>400</v>
+      </c>
+      <c r="C9" t="str">
+        <v>2025-05-14</v>
+      </c>
+      <c r="D9" t="str">
+        <v>Monthly electricity bill</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D9"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>